<commit_message>
update partlist and readme
</commit_message>
<xml_diff>
--- a/part_list/PartList_v2.xlsx
+++ b/part_list/PartList_v2.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10212"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/bin.yang/Work/Mypapers/supplement_repo/hr-lf-mv-SOLS/part_list/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DAA9A168-57EF-754C-BFA1-4ECA3DBFBC0F}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AEAE7B7B-01E1-2D4D-83D8-085E2970E1C8}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2880" yWindow="460" windowWidth="22720" windowHeight="15540" xr2:uid="{28437168-FD16-BA43-83EE-53029A5388A5}"/>
+    <workbookView xWindow="2880" yWindow="460" windowWidth="25340" windowHeight="20840" xr2:uid="{28437168-FD16-BA43-83EE-53029A5388A5}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -353,12 +353,6 @@
     <t>cDAQ-9178</t>
   </si>
   <si>
-    <t>NI-9262 DSUB</t>
-  </si>
-  <si>
-    <t>6 Ch, 1 MS/s/ch, 16-Bit AO C Series Module</t>
-  </si>
-  <si>
     <t xml:space="preserve"> 8-Channel, 100 ns, TTL Digital Input/Output Module</t>
   </si>
   <si>
@@ -438,9 +432,6 @@
   </si>
   <si>
     <t>Cage system</t>
-  </si>
-  <si>
-    <t>PAF2A15A</t>
   </si>
   <si>
     <t>FiberPort, FC/APC</t>
@@ -605,6 +596,15 @@
   </si>
   <si>
     <t>0.80NA 20x air objective</t>
+  </si>
+  <si>
+    <t>NI 9263 DSUB</t>
+  </si>
+  <si>
+    <t>4 Ch, +/-10 V, 16-Bit, 100 kS/s/ch,  AO Module</t>
+  </si>
+  <si>
+    <t>PAF2-A7A</t>
   </si>
 </sst>
 </file>
@@ -1021,8 +1021,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5BBF38FE-F0B2-A34F-8852-AEF1255FA0B8}">
   <dimension ref="A1:I83"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="86" zoomScaleNormal="86" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" topLeftCell="A12" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A24" sqref="A24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1040,14 +1040,14 @@
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.2">
       <c r="F1" s="11" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="G1" s="10">
         <f>SUM(G4:G103)</f>
-        <v>130700.97000000003</v>
+        <v>130568.35000000002</v>
       </c>
       <c r="H1" s="11" t="s">
-        <v>155</v>
+        <v>152</v>
       </c>
     </row>
     <row r="2" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -1110,13 +1110,13 @@
         <v>4</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>7</v>
       </c>
       <c r="D5" s="1" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="E5" s="3">
         <v>3075</v>
@@ -1153,7 +1153,7 @@
         <v>30000</v>
       </c>
       <c r="H6" s="1" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="7" spans="1:9" s="1" customFormat="1" ht="51" x14ac:dyDescent="0.2">
@@ -1210,7 +1210,7 @@
         <v>6288</v>
       </c>
       <c r="H8" s="1" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
     </row>
     <row r="9" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -1431,16 +1431,16 @@
     </row>
     <row r="18" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
+        <v>140</v>
+      </c>
+      <c r="B18" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="C18" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D18" s="1" t="s">
         <v>143</v>
-      </c>
-      <c r="B18" s="1" t="s">
-        <v>147</v>
-      </c>
-      <c r="C18" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D18" s="1" t="s">
-        <v>146</v>
       </c>
       <c r="E18" s="3">
         <v>496.7</v>
@@ -1453,21 +1453,21 @@
         <v>496.7</v>
       </c>
       <c r="H18" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="19" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B19" s="1" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C19" s="1" t="s">
         <v>74</v>
       </c>
       <c r="D19" s="1" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="E19" s="3">
         <v>731.3</v>
@@ -1480,21 +1480,21 @@
         <v>731.3</v>
       </c>
       <c r="H19" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="20" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B20" s="1" t="s">
-        <v>145</v>
+        <v>142</v>
       </c>
       <c r="C20" s="1" t="s">
         <v>74</v>
       </c>
       <c r="D20" s="1" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="E20" s="3">
         <v>818.85</v>
@@ -1507,7 +1507,7 @@
         <v>818.85</v>
       </c>
       <c r="H20" s="1" t="s">
-        <v>148</v>
+        <v>145</v>
       </c>
     </row>
     <row r="21" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
@@ -1536,7 +1536,7 @@
     </row>
     <row r="22" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>83</v>
@@ -1595,7 +1595,7 @@
     </row>
     <row r="26" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A26" s="2" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B26" s="5"/>
       <c r="C26" s="5"/>
@@ -1654,7 +1654,7 @@
         <v>24</v>
       </c>
       <c r="I28" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="29" spans="1:9" s="1" customFormat="1" ht="34" x14ac:dyDescent="0.2">
@@ -1734,23 +1734,23 @@
         <v>88</v>
       </c>
       <c r="B32" s="1" t="s">
-        <v>107</v>
+        <v>188</v>
       </c>
       <c r="C32" s="1" t="s">
         <v>103</v>
       </c>
       <c r="D32" s="1" t="s">
-        <v>106</v>
+        <v>187</v>
       </c>
       <c r="E32" s="3">
-        <v>1317</v>
+        <v>564</v>
       </c>
       <c r="F32" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G32" s="4">
         <f t="shared" si="1"/>
-        <v>1317</v>
+        <v>1128</v>
       </c>
     </row>
     <row r="33" spans="1:9" s="1" customFormat="1" ht="47" customHeight="1" x14ac:dyDescent="0.2">
@@ -1758,13 +1758,13 @@
         <v>88</v>
       </c>
       <c r="B33" s="1" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C33" s="1" t="s">
         <v>103</v>
       </c>
       <c r="D33" s="1" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="E33" s="3">
         <v>341</v>
@@ -1804,31 +1804,31 @@
         <v>99</v>
       </c>
       <c r="I34" s="1" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
     </row>
     <row r="35" spans="1:9" s="1" customFormat="1" ht="17" x14ac:dyDescent="0.2">
       <c r="A35" s="1" t="s">
-        <v>137</v>
+        <v>134</v>
       </c>
       <c r="B35" s="1" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C35" s="1" t="s">
         <v>74</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>135</v>
+        <v>189</v>
       </c>
       <c r="E35" s="8">
-        <v>569.74</v>
+        <v>626.12</v>
       </c>
       <c r="F35" s="1">
         <v>1</v>
       </c>
       <c r="G35" s="4">
         <f t="shared" si="1"/>
-        <v>569.74</v>
+        <v>626.12</v>
       </c>
     </row>
     <row r="36" spans="1:9" s="1" customFormat="1" x14ac:dyDescent="0.2">
@@ -2168,13 +2168,13 @@
     </row>
     <row r="54" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A54" s="1" t="s">
+        <v>115</v>
+      </c>
+      <c r="B54" t="s">
+        <v>116</v>
+      </c>
+      <c r="C54" s="1" t="s">
         <v>117</v>
-      </c>
-      <c r="B54" t="s">
-        <v>118</v>
-      </c>
-      <c r="C54" s="1" t="s">
-        <v>119</v>
       </c>
       <c r="D54" s="1" t="s">
         <v>47</v>
@@ -2194,7 +2194,7 @@
     </row>
     <row r="57" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A57" s="12" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
     </row>
     <row r="58" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -2251,16 +2251,16 @@
     </row>
     <row r="60" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A60" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B60" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C60" s="1" t="s">
         <v>74</v>
       </c>
       <c r="D60" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E60" s="3">
         <v>400.38</v>
@@ -2273,21 +2273,21 @@
         <v>1601.52</v>
       </c>
       <c r="H60" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
     </row>
     <row r="61" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A61" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B61" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="C61" s="1" t="s">
         <v>74</v>
       </c>
       <c r="D61" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="E61" s="3">
         <v>173.99</v>
@@ -2302,16 +2302,16 @@
     </row>
     <row r="62" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A62" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B62" t="s">
+        <v>125</v>
+      </c>
+      <c r="C62" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D62" t="s">
         <v>127</v>
-      </c>
-      <c r="C62" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D62" t="s">
-        <v>129</v>
       </c>
       <c r="E62" s="3">
         <v>147.29</v>
@@ -2326,16 +2326,16 @@
     </row>
     <row r="63" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A63" t="s">
+        <v>126</v>
+      </c>
+      <c r="B63" t="s">
+        <v>129</v>
+      </c>
+      <c r="C63" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D63" t="s">
         <v>128</v>
-      </c>
-      <c r="B63" t="s">
-        <v>131</v>
-      </c>
-      <c r="C63" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D63" t="s">
-        <v>130</v>
       </c>
       <c r="E63" s="3">
         <v>293.25</v>
@@ -2350,16 +2350,16 @@
     </row>
     <row r="64" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="B64" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="C64" s="1" t="s">
         <v>74</v>
       </c>
       <c r="D64" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="E64" s="3">
         <v>41.12</v>
@@ -2374,16 +2374,16 @@
     </row>
     <row r="65" spans="1:8" ht="34" x14ac:dyDescent="0.2">
       <c r="A65" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="B65" s="1" t="s">
-        <v>139</v>
+        <v>136</v>
       </c>
       <c r="C65" s="1" t="s">
         <v>74</v>
       </c>
       <c r="D65" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="E65" s="3">
         <v>223.78</v>
@@ -2398,16 +2398,16 @@
     </row>
     <row r="66" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>151</v>
+        <v>148</v>
       </c>
       <c r="B66" t="s">
-        <v>150</v>
+        <v>147</v>
       </c>
       <c r="C66" s="1" t="s">
         <v>74</v>
       </c>
       <c r="D66" t="s">
-        <v>149</v>
+        <v>146</v>
       </c>
       <c r="E66" s="3">
         <v>520.04999999999995</v>
@@ -2422,16 +2422,16 @@
     </row>
     <row r="67" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A67" t="s">
-        <v>154</v>
+        <v>151</v>
       </c>
       <c r="B67" t="s">
-        <v>153</v>
+        <v>150</v>
       </c>
       <c r="C67" s="1" t="s">
         <v>74</v>
       </c>
       <c r="D67" t="s">
-        <v>152</v>
+        <v>149</v>
       </c>
       <c r="E67" s="3">
         <v>120</v>
@@ -2446,16 +2446,16 @@
     </row>
     <row r="68" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B68" t="s">
-        <v>157</v>
+        <v>154</v>
       </c>
       <c r="C68" t="s">
         <v>74</v>
       </c>
       <c r="D68" t="s">
-        <v>156</v>
+        <v>153</v>
       </c>
       <c r="E68" s="3">
         <v>25.97</v>
@@ -2470,16 +2470,16 @@
     </row>
     <row r="69" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
+        <v>155</v>
+      </c>
+      <c r="B69" t="s">
+        <v>157</v>
+      </c>
+      <c r="C69" t="s">
+        <v>74</v>
+      </c>
+      <c r="D69" t="s">
         <v>158</v>
-      </c>
-      <c r="B69" t="s">
-        <v>160</v>
-      </c>
-      <c r="C69" t="s">
-        <v>74</v>
-      </c>
-      <c r="D69" t="s">
-        <v>161</v>
       </c>
       <c r="E69" s="3">
         <v>33.28</v>
@@ -2494,16 +2494,16 @@
     </row>
     <row r="70" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A70" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="B70" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="C70" t="s">
         <v>74</v>
       </c>
       <c r="D70" t="s">
-        <v>159</v>
+        <v>156</v>
       </c>
       <c r="E70" s="3">
         <v>23.27</v>
@@ -2518,16 +2518,16 @@
     </row>
     <row r="71" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A71" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="B71" t="s">
-        <v>164</v>
+        <v>161</v>
       </c>
       <c r="C71" s="1" t="s">
         <v>74</v>
       </c>
       <c r="D71" t="s">
-        <v>163</v>
+        <v>160</v>
       </c>
       <c r="E71" s="3">
         <v>37.869999999999997</v>
@@ -2540,21 +2540,21 @@
         <v>113.60999999999999</v>
       </c>
       <c r="H71" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="72" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A72" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B72" t="s">
-        <v>167</v>
+        <v>164</v>
       </c>
       <c r="C72" s="1" t="s">
         <v>74</v>
       </c>
       <c r="D72" t="s">
-        <v>166</v>
+        <v>163</v>
       </c>
       <c r="E72" s="3">
         <v>427.54</v>
@@ -2567,21 +2567,21 @@
         <v>427.54</v>
       </c>
       <c r="H72" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="73" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A73" t="s">
-        <v>168</v>
+        <v>165</v>
       </c>
       <c r="B73" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C73" s="1" t="s">
         <v>74</v>
       </c>
       <c r="D73" t="s">
-        <v>170</v>
+        <v>167</v>
       </c>
       <c r="E73" s="3">
         <v>32.619999999999997</v>
@@ -2594,21 +2594,21 @@
         <v>32.619999999999997</v>
       </c>
       <c r="H73" t="s">
-        <v>165</v>
+        <v>162</v>
       </c>
     </row>
     <row r="74" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A74" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B74" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C74" s="1" t="s">
         <v>74</v>
       </c>
       <c r="D74" t="s">
-        <v>172</v>
+        <v>169</v>
       </c>
       <c r="E74" s="3">
         <v>74.900000000000006</v>
@@ -2621,21 +2621,21 @@
         <v>74.900000000000006</v>
       </c>
       <c r="H74" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="75" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A75" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B75" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C75" s="1" t="s">
         <v>74</v>
       </c>
       <c r="D75" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
       <c r="E75" s="3">
         <v>187.83</v>
@@ -2648,21 +2648,21 @@
         <v>187.83</v>
       </c>
       <c r="H75" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="76" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A76" t="s">
+        <v>168</v>
+      </c>
+      <c r="B76" t="s">
+        <v>178</v>
+      </c>
+      <c r="C76" s="1" t="s">
+        <v>74</v>
+      </c>
+      <c r="D76" t="s">
         <v>171</v>
-      </c>
-      <c r="B76" t="s">
-        <v>181</v>
-      </c>
-      <c r="C76" s="1" t="s">
-        <v>74</v>
-      </c>
-      <c r="D76" t="s">
-        <v>174</v>
       </c>
       <c r="E76" s="3">
         <v>129.11000000000001</v>
@@ -2675,21 +2675,21 @@
         <v>129.11000000000001</v>
       </c>
       <c r="H76" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="77" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A77" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B77" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C77" s="1" t="s">
         <v>74</v>
       </c>
       <c r="D77" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="E77" s="3">
         <v>375.66</v>
@@ -2702,21 +2702,21 @@
         <v>375.66</v>
       </c>
       <c r="H77" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="78" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A78" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B78" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C78" s="1" t="s">
         <v>74</v>
       </c>
       <c r="D78" t="s">
-        <v>176</v>
+        <v>173</v>
       </c>
       <c r="E78" s="3">
         <v>568.64</v>
@@ -2729,21 +2729,21 @@
         <v>568.64</v>
       </c>
       <c r="H78" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="79" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A79" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B79" t="s">
-        <v>181</v>
+        <v>178</v>
       </c>
       <c r="C79" s="1" t="s">
         <v>74</v>
       </c>
       <c r="D79" t="s">
-        <v>177</v>
+        <v>174</v>
       </c>
       <c r="E79" s="3">
         <v>115.16</v>
@@ -2756,21 +2756,21 @@
         <v>115.16</v>
       </c>
       <c r="H79" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="80" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A80" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B80" t="s">
-        <v>179</v>
+        <v>176</v>
       </c>
       <c r="C80" s="1" t="s">
         <v>74</v>
       </c>
       <c r="D80" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="E80" s="3">
         <v>83.71</v>
@@ -2783,21 +2783,21 @@
         <v>251.13</v>
       </c>
       <c r="H80" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="81" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A81" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B81" t="s">
-        <v>187</v>
+        <v>184</v>
       </c>
       <c r="C81" s="1" t="s">
         <v>74</v>
       </c>
       <c r="D81" t="s">
-        <v>180</v>
+        <v>177</v>
       </c>
       <c r="E81" s="3">
         <v>164.27</v>
@@ -2810,21 +2810,21 @@
         <v>164.27</v>
       </c>
       <c r="H81" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="82" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A82" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="B82" t="s">
-        <v>186</v>
+        <v>183</v>
       </c>
       <c r="C82" s="1" t="s">
         <v>74</v>
       </c>
       <c r="D82" t="s">
-        <v>182</v>
+        <v>179</v>
       </c>
       <c r="E82" s="3">
         <v>129.11000000000001</v>
@@ -2837,21 +2837,21 @@
         <v>387.33000000000004</v>
       </c>
       <c r="H82" t="s">
-        <v>188</v>
+        <v>185</v>
       </c>
     </row>
     <row r="83" spans="1:8" ht="17" x14ac:dyDescent="0.2">
       <c r="A83" t="s">
-        <v>185</v>
+        <v>182</v>
       </c>
       <c r="B83" t="s">
-        <v>184</v>
+        <v>181</v>
       </c>
       <c r="C83" s="1" t="s">
         <v>74</v>
       </c>
       <c r="D83" t="s">
-        <v>183</v>
+        <v>180</v>
       </c>
       <c r="E83" s="3">
         <v>374.58</v>

</xml_diff>